<commit_message>
Add a system to schedule and track equipment maintenance and repairs
Implements maintenance scheduling using models in `models/maintenance.py`, routes in `routes/maintenance.py`, and templates in `templates/maintenance.html` and `templates/maintenance_schedules.html`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/bfa7266b-80ad-4f4f-a4be-217b575c7b39.jpg
</commit_message>
<xml_diff>
--- a/reports/2025-05-16/prior_day_report_2025-05-15.xlsx
+++ b/reports/2025-05-16/prior_day_report_2025-05-15.xlsx
@@ -510,7 +510,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,10 +520,10 @@
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
     <col width="26" customWidth="1" min="2" max="2"/>
-    <col width="32" customWidth="1" min="3" max="3"/>
+    <col width="26" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="26" customWidth="1" min="6" max="6"/>
+    <col width="23" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
@@ -999,182 +999,6 @@
         </is>
       </c>
       <c r="R9" s="7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="5" t="inlineStr">
-        <is>
-          <t>VICK ADHIKARI</t>
-        </is>
-      </c>
-      <c r="B10" s="5" t="inlineStr">
-        <is>
-          <t>2023-006</t>
-        </is>
-      </c>
-      <c r="C10" s="5" t="inlineStr">
-        <is>
-          <t>Tarrant SH 183 Bridge Replacem</t>
-        </is>
-      </c>
-      <c r="D10" s="5" t="inlineStr">
-        <is>
-          <t>ET-01</t>
-        </is>
-      </c>
-      <c r="E10" s="5" t="inlineStr">
-        <is>
-          <t>210074</t>
-        </is>
-      </c>
-      <c r="F10" s="5" t="inlineStr">
-        <is>
-          <t>Martinez Alvarez, Saul</t>
-        </is>
-      </c>
-      <c r="G10" s="5" t="inlineStr"/>
-      <c r="H10" s="5" t="inlineStr">
-        <is>
-          <t>Arrived</t>
-        </is>
-      </c>
-      <c r="I10" s="5" t="inlineStr">
-        <is>
-          <t>Departed</t>
-        </is>
-      </c>
-      <c r="J10" s="5" t="inlineStr">
-        <is>
-          <t>2023-006</t>
-        </is>
-      </c>
-      <c r="K10" s="5" t="inlineStr">
-        <is>
-          <t>7:00 AM</t>
-        </is>
-      </c>
-      <c r="L10" s="5" t="inlineStr">
-        <is>
-          <t>5:30 PM</t>
-        </is>
-      </c>
-      <c r="M10" s="6" t="inlineStr">
-        <is>
-          <t>Late</t>
-        </is>
-      </c>
-      <c r="N10" s="6" t="inlineStr">
-        <is>
-          <t>Left Early</t>
-        </is>
-      </c>
-      <c r="O10" s="5" t="inlineStr">
-        <is>
-          <t>7:05 AM</t>
-        </is>
-      </c>
-      <c r="P10" s="5" t="inlineStr">
-        <is>
-          <t>5:18 PM</t>
-        </is>
-      </c>
-      <c r="Q10" s="5" t="inlineStr">
-        <is>
-          <t>6:50:00</t>
-        </is>
-      </c>
-      <c r="R10" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="7" t="inlineStr">
-        <is>
-          <t>VICK ADHIKARI</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>2024-004</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="inlineStr">
-        <is>
-          <t>City of Dallas Sidewalk 2024</t>
-        </is>
-      </c>
-      <c r="D11" s="7" t="inlineStr">
-        <is>
-          <t>PT-09S</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="inlineStr">
-        <is>
-          <t>ESPJOV</t>
-        </is>
-      </c>
-      <c r="F11" s="7" t="inlineStr">
-        <is>
-          <t>Espinoza-Casillas, Jovan</t>
-        </is>
-      </c>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="7" t="inlineStr">
-        <is>
-          <t>Arrived</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr">
-        <is>
-          <t>Departed</t>
-        </is>
-      </c>
-      <c r="J11" s="7" t="inlineStr">
-        <is>
-          <t>24-04</t>
-        </is>
-      </c>
-      <c r="K11" s="7" t="inlineStr">
-        <is>
-          <t>7:00 AM</t>
-        </is>
-      </c>
-      <c r="L11" s="7" t="inlineStr">
-        <is>
-          <t>5:30 PM</t>
-        </is>
-      </c>
-      <c r="M11" s="8" t="inlineStr">
-        <is>
-          <t>Late</t>
-        </is>
-      </c>
-      <c r="N11" s="8" t="inlineStr">
-        <is>
-          <t>Left Early</t>
-        </is>
-      </c>
-      <c r="O11" s="7" t="inlineStr">
-        <is>
-          <t>7:26 AM</t>
-        </is>
-      </c>
-      <c r="P11" s="7" t="inlineStr">
-        <is>
-          <t>12:52 PM</t>
-        </is>
-      </c>
-      <c r="Q11" s="7" t="inlineStr">
-        <is>
-          <t>4:23:00</t>
-        </is>
-      </c>
-      <c r="R11" s="7" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>